<commit_message>
edited FP and added TestPlan(only structure)
</commit_message>
<xml_diff>
--- a/FunctionPoints/FP-UseCases.xlsx
+++ b/FunctionPoints/FP-UseCases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorenz Seufert\Documents\Studium Angewandte Informatik\Projekt CeangalMessenger\FunctionPoints\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorenz Seufert\IdeaProjects\CeangalMessenger---Documentation\FunctionPoints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3250FEE-745D-4C30-8D28-15FD17AEC682}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B54430-12FE-490C-899F-3639A12155ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AF518DA0-E955-4FB1-ABA7-5E86C6F23D2E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="76">
   <si>
     <t>Function points</t>
   </si>
@@ -247,6 +247,21 @@
   </si>
   <si>
     <t>Show friends</t>
+  </si>
+  <si>
+    <t>Old</t>
+  </si>
+  <si>
+    <t>With function</t>
+  </si>
+  <si>
+    <t>Send private text</t>
+  </si>
+  <si>
+    <t>Edit text channel</t>
+  </si>
+  <si>
+    <t>Delete account</t>
   </si>
 </sst>
 </file>
@@ -584,12 +599,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
@@ -602,6 +611,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -634,6 +649,14 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.33709711286089239"/>
+          <c:y val="0"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -665,21 +688,26 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.5025371828521417E-2"/>
+          <c:y val="0.18560185185185185"/>
+          <c:w val="0.90286351706036749"/>
+          <c:h val="0.72088764946048411"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>FP</c:v>
-          </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -699,40 +727,75 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Tabelle1!$M$8:$M$12</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>Show friends</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Add friend</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Edit user profile</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Create user profile</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Create text channel</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="de-DE"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
             <c:numRef>
               <c:f>Tabelle1!$N$8:$N$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>16.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26.4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>44</c:v>
@@ -741,82 +804,22 @@
                   <c:v>49.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>84.7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9E5C-44B2-8C1D-9A5993C9FC15}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Time</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Tabelle1!$M$8:$M$12</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>Show friends</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Add friend</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Edit user profile</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Create user profile</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Create text channel</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Tabelle1!$O$8:$O$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4</c:v>
@@ -825,15 +828,15 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-9E5C-44B2-8C1D-9A5993C9FC15}"/>
+              <c16:uniqueId val="{00000000-22E2-407A-ACD1-E2DFA291F96D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -845,18 +848,30 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="1236224175"/>
-        <c:axId val="1236224591"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="1236224175"/>
+        <c:axId val="91404463"/>
+        <c:axId val="91396975"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="91404463"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -866,8 +881,8 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -894,15 +909,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1236224591"/>
+        <c:crossAx val="91396975"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="1236224591"/>
+        <c:axId val="91396975"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -928,8 +940,14 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -953,9 +971,9 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1236224175"/>
+        <c:crossAx val="91404463"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -965,46 +983,8 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -1035,7 +1015,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -1081,7 +1061,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1108,8 +1088,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1210,7 +1190,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1242,10 +1222,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1285,22 +1265,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -1405,8 +1386,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1538,19 +1519,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1564,6 +1546,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -1587,23 +1580,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>100012</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>714375</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>719137</xdr:colOff>
+      <xdr:colOff>571500</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="10" name="Diagramm 9">
+        <xdr:cNvPr id="2" name="Diagramm 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F21ECF6-E297-4DE4-9962-D1564EDA81CB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D748253-7A0E-4D2F-8B32-BA9CDBAC213D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1923,8 +1916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFF1C0A3-8DC3-475E-A9A2-E80B60369D51}">
   <dimension ref="A1:O70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="Q43" sqref="Q43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1937,6 +1930,7 @@
     <col min="7" max="7" width="2.5703125" customWidth="1"/>
     <col min="8" max="8" width="16.42578125" customWidth="1"/>
     <col min="9" max="9" width="3" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" customWidth="1"/>
     <col min="13" max="13" width="18.85546875" customWidth="1"/>
     <col min="14" max="14" width="14.28515625" customWidth="1"/>
     <col min="15" max="15" width="14.7109375" customWidth="1"/>
@@ -2017,13 +2011,13 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="8"/>
-      <c r="M7" s="13" t="s">
+      <c r="M7" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="N7" s="14" t="s">
+      <c r="N7" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="O7" s="15" t="s">
+      <c r="O7" s="13" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2047,14 +2041,14 @@
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="8"/>
-      <c r="M8" s="16" t="s">
+      <c r="M8" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="N8" s="17">
-        <v>16.5</v>
-      </c>
-      <c r="O8" s="18">
-        <v>1.5</v>
+      <c r="N8" s="15">
+        <v>0</v>
+      </c>
+      <c r="O8" s="16">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2085,14 +2079,14 @@
       <c r="I9" s="8">
         <v>1</v>
       </c>
-      <c r="M9" s="19" t="s">
+      <c r="M9" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="N9" s="20">
-        <v>26.4</v>
-      </c>
-      <c r="O9" s="21">
-        <v>3</v>
+      <c r="N9" s="18">
+        <v>0</v>
+      </c>
+      <c r="O9" s="19">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2123,13 +2117,13 @@
       <c r="I10" s="8">
         <v>1</v>
       </c>
-      <c r="M10" s="19" t="s">
+      <c r="M10" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="N10" s="20">
+      <c r="N10" s="18">
         <v>44</v>
       </c>
-      <c r="O10" s="21">
+      <c r="O10" s="19">
         <v>4</v>
       </c>
     </row>
@@ -2137,35 +2131,35 @@
       <c r="A11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="23">
         <v>26.4</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="12"/>
-      <c r="M11" s="19" t="s">
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="24"/>
+      <c r="M11" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="N11" s="20">
+      <c r="N11" s="18">
         <v>49.5</v>
       </c>
-      <c r="O11" s="21">
+      <c r="O11" s="19">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M12" s="22" t="s">
+      <c r="M12" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="N12" s="23">
-        <v>84.7</v>
-      </c>
-      <c r="O12" s="24">
-        <v>7</v>
+      <c r="N12" s="21">
+        <v>0</v>
+      </c>
+      <c r="O12" s="22">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -2278,7 +2272,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>5</v>
       </c>
@@ -2307,7 +2301,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>6</v>
       </c>
@@ -2336,23 +2330,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="11">
+      <c r="B19" s="23">
         <v>84.7</v>
       </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="12"/>
-    </row>
-    <row r="20" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="24"/>
+    </row>
+    <row r="20" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>38</v>
       </c>
@@ -2375,7 +2369,7 @@
       </c>
       <c r="I21" s="6"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>2</v>
       </c>
@@ -2404,7 +2398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>3</v>
       </c>
@@ -2417,7 +2411,7 @@
       <c r="H23" s="3"/>
       <c r="I23" s="8"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>4</v>
       </c>
@@ -2446,7 +2440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>5</v>
       </c>
@@ -2475,7 +2469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>6</v>
       </c>
@@ -2504,23 +2498,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="11">
+      <c r="B27" s="23">
         <v>49.5</v>
       </c>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="12"/>
-    </row>
-    <row r="28" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="24"/>
+    </row>
+    <row r="28" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>15</v>
       </c>
@@ -2543,7 +2537,7 @@
       </c>
       <c r="I29" s="6"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>2</v>
       </c>
@@ -2572,7 +2566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>3</v>
       </c>
@@ -2600,8 +2594,18 @@
       <c r="I31" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L31" t="s">
+        <v>71</v>
+      </c>
+      <c r="M31" s="11"/>
+      <c r="N31" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="O31" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>4</v>
       </c>
@@ -2629,8 +2633,18 @@
       <c r="I32" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M32" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="N32" s="15">
+        <v>16.5</v>
+      </c>
+      <c r="O32" s="16">
+        <f>(0.0967*N32)-0.0092</f>
+        <v>1.5863499999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>5</v>
       </c>
@@ -2658,8 +2672,17 @@
       <c r="I33" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M33" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="N33" s="18">
+        <v>26.4</v>
+      </c>
+      <c r="O33" s="19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>6</v>
       </c>
@@ -2687,32 +2710,59 @@
       <c r="I34" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M34" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="N34" s="18">
+        <v>44</v>
+      </c>
+      <c r="O34" s="19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B35" s="11">
+      <c r="B35" s="23">
         <v>44</v>
       </c>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="12"/>
-    </row>
-    <row r="36" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C35" s="23"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="23"/>
+      <c r="I35" s="24"/>
+      <c r="M35" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="N35" s="18">
+        <v>49.5</v>
+      </c>
+      <c r="O35" s="19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M36" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="N36" s="21">
+        <v>84.7</v>
+      </c>
+      <c r="O36" s="22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>17</v>
       </c>
@@ -2734,8 +2784,18 @@
         <v>12</v>
       </c>
       <c r="I39" s="6"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L39" t="s">
+        <v>72</v>
+      </c>
+      <c r="M39" s="11"/>
+      <c r="N39" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="O39" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>2</v>
       </c>
@@ -2761,8 +2821,18 @@
       <c r="I40" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M40" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="N40" s="15">
+        <v>16.5</v>
+      </c>
+      <c r="O40" s="16">
+        <f>(0.0967*N40)-0.0092</f>
+        <v>1.5863499999999997</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>3</v>
       </c>
@@ -2790,8 +2860,18 @@
       <c r="I41" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M41" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="N41" s="18">
+        <v>26.4</v>
+      </c>
+      <c r="O41" s="19">
+        <f>(0.0967*N41)-0.0092</f>
+        <v>2.5436799999999997</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>4</v>
       </c>
@@ -2819,8 +2899,17 @@
       <c r="I42" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M42" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="N42" s="18">
+        <v>44</v>
+      </c>
+      <c r="O42" s="19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>5</v>
       </c>
@@ -2832,8 +2921,18 @@
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
       <c r="I43" s="8"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M43" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="N43" s="18">
+        <v>49.5</v>
+      </c>
+      <c r="O43" s="19">
+        <f>(0.0967*N43)-0.0092</f>
+        <v>4.77745</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>6</v>
       </c>
@@ -2861,24 +2960,55 @@
       <c r="I44" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M44" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="N44" s="21">
+        <v>84.7</v>
+      </c>
+      <c r="O44" s="22">
+        <f>(0.0967*N44)-0.0092</f>
+        <v>8.1812900000000006</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B45" s="11">
+      <c r="B45" s="23">
         <v>16.5</v>
       </c>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
-      <c r="I45" s="12"/>
-    </row>
-    <row r="46" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C45" s="23"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="23"/>
+      <c r="F45" s="23"/>
+      <c r="G45" s="23"/>
+      <c r="H45" s="23"/>
+      <c r="I45" s="24"/>
+      <c r="M45" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="N45" s="21">
+        <v>53.9</v>
+      </c>
+      <c r="O45" s="22">
+        <f t="shared" ref="O45:O47" si="0">(0.0967*N45)-0.0092</f>
+        <v>5.2029299999999994</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M46" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="N46" s="21">
+        <v>48.4</v>
+      </c>
+      <c r="O46" s="22">
+        <f t="shared" si="0"/>
+        <v>4.6710799999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>18</v>
       </c>
@@ -2900,8 +3030,18 @@
         <v>12</v>
       </c>
       <c r="I47" s="6"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M47" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="N47" s="21">
+        <v>33</v>
+      </c>
+      <c r="O47" s="22">
+        <f t="shared" si="0"/>
+        <v>3.1818999999999997</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>2</v>
       </c>
@@ -3050,16 +3190,16 @@
       <c r="A53" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B53" s="11">
+      <c r="B53" s="23">
         <v>53.9</v>
       </c>
-      <c r="C53" s="11"/>
-      <c r="D53" s="11"/>
-      <c r="E53" s="11"/>
-      <c r="F53" s="11"/>
-      <c r="G53" s="11"/>
-      <c r="H53" s="11"/>
-      <c r="I53" s="12"/>
+      <c r="C53" s="23"/>
+      <c r="D53" s="23"/>
+      <c r="E53" s="23"/>
+      <c r="F53" s="23"/>
+      <c r="G53" s="23"/>
+      <c r="H53" s="23"/>
+      <c r="I53" s="24"/>
     </row>
     <row r="54" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="55" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -3234,16 +3374,16 @@
       <c r="A61" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B61" s="11">
+      <c r="B61" s="23">
         <v>48.4</v>
       </c>
-      <c r="C61" s="11"/>
-      <c r="D61" s="11"/>
-      <c r="E61" s="11"/>
-      <c r="F61" s="11"/>
-      <c r="G61" s="11"/>
-      <c r="H61" s="11"/>
-      <c r="I61" s="12"/>
+      <c r="C61" s="23"/>
+      <c r="D61" s="23"/>
+      <c r="E61" s="23"/>
+      <c r="F61" s="23"/>
+      <c r="G61" s="23"/>
+      <c r="H61" s="23"/>
+      <c r="I61" s="24"/>
     </row>
     <row r="62" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="63" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -3402,16 +3542,16 @@
       <c r="A69" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B69" s="11">
+      <c r="B69" s="23">
         <v>33</v>
       </c>
-      <c r="C69" s="11"/>
-      <c r="D69" s="11"/>
-      <c r="E69" s="11"/>
-      <c r="F69" s="11"/>
-      <c r="G69" s="11"/>
-      <c r="H69" s="11"/>
-      <c r="I69" s="12"/>
+      <c r="C69" s="23"/>
+      <c r="D69" s="23"/>
+      <c r="E69" s="23"/>
+      <c r="F69" s="23"/>
+      <c r="G69" s="23"/>
+      <c r="H69" s="23"/>
+      <c r="I69" s="24"/>
     </row>
     <row r="70" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>

</xml_diff>